<commit_message>
Switched to strict typing and updated as needed
</commit_message>
<xml_diff>
--- a/Winners.xlsx
+++ b/Winners.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="10">
   <si>
     <t>Order</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>0xdAFf0e93f8614D42Ae3Efa26657587Cd4d4bBc21</t>
+  </si>
+  <si>
+    <t>Jon3</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -411,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D30"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -736,6 +742,104 @@
         <v>7</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>